<commit_message>
Refactoring Erythyro & Ichthama
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-amdo-side-data.xlsx
+++ b/tabular/eve/epv-amdo-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3004DB4B-4E81-1A46-96FB-B14DE4D2FBD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1733C57-D985-EF4D-9400-2442D3205EB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19720" yWindow="2720" windowWidth="31140" windowHeight="26000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection sqref="A1:AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1888,7 +1888,7 @@
         <v>102</v>
       </c>
       <c r="C8" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>97</v>

</xml_diff>